<commit_message>
fixed error in computing for total
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Joson,Alfonso Miguel.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Joson,Alfonso Miguel.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="67">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -50,61 +50,127 @@
     <t>REMARKS</t>
   </si>
   <si>
-    <t>02-10-2015</t>
+    <t>04-04-2015</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Others|Mydin Barter-SAP Go Live|</t>
+  </si>
+  <si>
+    <t>04-05-2015</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>04-06-2015</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>04-07-2015</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>" Others|Mydin SAP Integration, Support|"</t>
-  </si>
-  <si>
-    <t>02-11-2015</t>
+    <t>04-08-2015</t>
   </si>
   <si>
     <t>Wednesday</t>
   </si>
   <si>
-    <t>02-12-2015</t>
+    <t>04-09-2015</t>
   </si>
   <si>
     <t>Thursday</t>
   </si>
   <si>
-    <t>02-13-2015</t>
+    <t>04-10-2015</t>
   </si>
   <si>
     <t>Friday</t>
   </si>
   <si>
-    <t>02-14-2015</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>02-15-2015</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>02-16-2015</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>02-17-2015</t>
-  </si>
-  <si>
-    <t>02-18-2015</t>
-  </si>
-  <si>
-    <t>02-19-2015</t>
-  </si>
-  <si>
-    <t>02-20-2015</t>
+    <t>04-11-2015</t>
+  </si>
+  <si>
+    <t>04-12-2015</t>
+  </si>
+  <si>
+    <t>04-13-2015</t>
+  </si>
+  <si>
+    <t>04-14-2015</t>
+  </si>
+  <si>
+    <t>04-15-2015</t>
+  </si>
+  <si>
+    <t>04-16-2015</t>
+  </si>
+  <si>
+    <t>04-17-2015</t>
+  </si>
+  <si>
+    <t>08:46:00</t>
+  </si>
+  <si>
+    <t>18:26:00</t>
+  </si>
+  <si>
+    <t>04-18-2015</t>
+  </si>
+  <si>
+    <t>08:19:00</t>
+  </si>
+  <si>
+    <t>18:05:00</t>
+  </si>
+  <si>
+    <t>04-19-2015</t>
+  </si>
+  <si>
+    <t>04-20-2015</t>
+  </si>
+  <si>
+    <t>08:09:00</t>
+  </si>
+  <si>
+    <t>18:47:00</t>
+  </si>
+  <si>
+    <t>04-21-2015</t>
+  </si>
+  <si>
+    <t>08:07:00</t>
+  </si>
+  <si>
+    <t>18:44:00</t>
+  </si>
+  <si>
+    <t>04-22-2015</t>
+  </si>
+  <si>
+    <t>08:26:00</t>
+  </si>
+  <si>
+    <t>18:39:00</t>
+  </si>
+  <si>
+    <t>04-23-2015</t>
+  </si>
+  <si>
+    <t>08:20:00</t>
+  </si>
+  <si>
+    <t>04-24-2015</t>
+  </si>
+  <si>
+    <t>08:39:00</t>
   </si>
   <si>
     <t>NUMBER OF TIMES TARDY</t>
@@ -341,7 +407,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -356,7 +422,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="34.33483146067415"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="24.434831460674157"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="17.834831460674156"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="43.789887640449436"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="26.18988764044944"/>
     <col min="11" max="11" bestFit="false" customWidth="false" hidden="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="4.189887640449439" hidden="true"/>
     <col min="13" max="13" bestFit="false" customWidth="false" hidden="true"/>
@@ -676,449 +742,733 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="str">
-        <f>COUNT(F5:F15)</f>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <f>SUM(F5:F15)</f>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>33</v>
+      <c r="B17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="5" t="str">
-        <f>SUM(G5:G15)</f>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J18" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="5" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="5" t="str">
-        <f>SUM(H5:H15)</f>
-      </c>
-      <c r="I19" s="5" t="str">
-        <f>SUM(I5:I15)</f>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20"/>
+        <v>39</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J19" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I20" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <f>FLOOR(G18/8,1)&amp;"."&amp;FLOOR(MOD(G18,8),1)&amp;"."&amp;(MOD(G18,8)-FLOOR(MOD(G18,8),1))*60</f>
+        <v>41</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K21" s="5" t="str">
-        <f>INT(LEFT(B22,1))</f>
-      </c>
-      <c r="L21" s="5" t="str">
-        <f>RIGHT(B22,LEN(B22)-2)</f>
-      </c>
-      <c r="M21" s="5" t="str">
-        <f>INT(LEFT(L21,1))</f>
-      </c>
-      <c r="N21" s="5" t="str">
-        <f>RIGHT(L21,LEN(L21)-2)+0</f>
-      </c>
-      <c r="O21" s="5" t="str">
-        <f>K21*8*60+M21*60+N21</f>
+        <v>43</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H21" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I21" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J21" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="5" t="str">
-        <f>FLOOR(F17/8,1)&amp;"."&amp;FLOOR(MOD(F17,8),1)&amp;"."&amp;(MOD(F17,8)-FLOOR(MOD(F17,8),1))*60</f>
+        <v>44</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="5" t="str">
-        <f>INT(LEFT(B23,1))</f>
-      </c>
-      <c r="L22" s="5" t="str">
-        <f>RIGHT(B23,LEN(B23)-2)</f>
-      </c>
-      <c r="M22" s="5" t="str">
-        <f>INT(LEFT(L22,1))</f>
-      </c>
-      <c r="N22" s="5" t="str">
-        <f>RIGHT(L22,LEN(L22)-2)+0</f>
-      </c>
-      <c r="O22" s="5" t="str">
-        <f>K22*8*60+M22*60+N22</f>
+        <v>46</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I22" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J22" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <f>FLOOR(H19,1)&amp;"."&amp;(H19-FLOOR(H19,1))*8&amp;".0"</f>
+        <v>47</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K23" s="5" t="str">
-        <f>INT(LEFT(B24,1))</f>
-      </c>
-      <c r="L23" s="5" t="str">
-        <f>RIGHT(B24,LEN(B24)-2)</f>
-      </c>
-      <c r="M23" s="5" t="str">
-        <f>INT(LEFT(L23,1))</f>
-      </c>
-      <c r="N23" s="5" t="str">
-        <f>RIGHT(L23,LEN(L23)-2)+0</f>
-      </c>
-      <c r="O23" s="5" t="str">
-        <f>K23*8*60+M23*60+N23</f>
+        <v>49</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J23" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="5" t="str">
-        <f>FLOOR(I19,1)&amp;"."&amp;(I19-FLOOR(I19,1))*8&amp;".0"</f>
+        <v>50</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K24" s="5" t="str">
-        <f>INT(LEFT(B25,1))</f>
-      </c>
-      <c r="L24" s="5" t="str">
-        <f>RIGHT(B25,LEN(B25)-2)</f>
-      </c>
-      <c r="M24" s="5" t="str">
-        <f>INT(LEFT(L24,1))</f>
-      </c>
-      <c r="N24" s="5" t="str">
-        <f>RIGHT(L24,LEN(L24)-2)+0</f>
-      </c>
-      <c r="O24" s="5" t="str">
-        <f>K24*8*60+M24*60+N24</f>
+        <v>51</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I24" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J24" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K25" s="5" t="str">
-        <f>INT(LEFT(B26,1))</f>
-      </c>
-      <c r="L25" s="5" t="str">
-        <f>RIGHT(B26,LEN(B26)-2)</f>
-      </c>
-      <c r="M25" s="5" t="str">
-        <f>INT(LEFT(L25,1))</f>
-      </c>
-      <c r="N25" s="5" t="str">
-        <f>RIGHT(L25,LEN(L25)-2)+0</f>
-      </c>
-      <c r="O25" s="5" t="str">
-        <f>K25*8*60+M25*60+N25</f>
+        <v>53</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I25" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J25" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
+      </c>
+      <c r="F26" s="5" t="str">
+        <f>COUNT(F5:F25)</f>
       </c>
       <c r="G26" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K26" s="5" t="str">
-        <f>K21+IF(K22&gt;K24,K22-K24,0)+IF(K23&gt;K25,K23-K25,0)</f>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M26" s="5" t="str">
-        <f>M21+IF(M22&gt;M24,M22-M24,0)+IF(M23&gt;M25,M23-M25,0)</f>
-      </c>
-      <c r="N26" s="5" t="str">
-        <f>N21+IF(N22&gt;N24,N22-N24,0)+IF(N23&gt;N25,N23-N25,0)</f>
-      </c>
-      <c r="O26" s="5" t="str">
-        <f>O21+IF(O22&gt;O24,O22-O24,0)+IF(O23&gt;O25,O23-O25,0)</f>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="5" t="str">
-        <f>FLOOR(K27/8,1)&amp;"."&amp;FLOOR(MOD(K27,8),1)&amp;"."&amp;(MOD(K27,8)-FLOOR(MOD(K27,8),1))*60</f>
+        <v>56</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
+      </c>
+      <c r="F27" s="5" t="str">
+        <f>SUM(F5:F25)</f>
       </c>
       <c r="G27" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27" s="5" t="str">
-        <f>O26/60</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="5" t="str">
+        <f>SUM(G5:G25)</f>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="5" t="str">
+        <f>SUM(H5:H25)</f>
+      </c>
+      <c r="I29" s="5" t="str">
+        <f>SUM(I5:I25)</f>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="A31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <f>FLOOR(G28/8,1)&amp;"."&amp;FLOOR(MOD(G28,8),1)&amp;"."&amp;(MOD(G28,8)-FLOOR(MOD(G28,8),1))*60</f>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K31" s="5" t="str">
+        <f>INT(LEFT(B32,1))</f>
+      </c>
+      <c r="L31" s="5" t="str">
+        <f>RIGHT(B32,LEN(B32)-2)</f>
+      </c>
+      <c r="M31" s="5" t="str">
+        <f>INT(LEFT(L31,1))</f>
+      </c>
+      <c r="N31" s="5" t="str">
+        <f>RIGHT(L31,LEN(L31)-2)+0</f>
+      </c>
+      <c r="O31" s="5" t="str">
+        <f>K31*8*60+M31*60+N31</f>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="5" t="str">
+        <f>FLOOR(F27/8,1)&amp;"."&amp;FLOOR(MOD(F27,8),1)&amp;"."&amp;(MOD(F27,8)-FLOOR(MOD(F27,8),1))*60</f>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K32" s="5" t="str">
+        <f>INT(LEFT(B33,1))</f>
+      </c>
+      <c r="L32" s="5" t="str">
+        <f>RIGHT(B33,LEN(B33)-2)</f>
+      </c>
+      <c r="M32" s="5" t="str">
+        <f>INT(LEFT(L32,1))</f>
+      </c>
+      <c r="N32" s="5" t="str">
+        <f>RIGHT(L32,LEN(L32)-2)+0</f>
+      </c>
+      <c r="O32" s="5" t="str">
+        <f>K32*8*60+M32*60+N32</f>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <f>FLOOR(H29,1)&amp;"."&amp;(H29-FLOOR(H29,1))*8&amp;".0"</f>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K33" s="5" t="str">
+        <f>INT(LEFT(B34,1))</f>
+      </c>
+      <c r="L33" s="5" t="str">
+        <f>RIGHT(B34,LEN(B34)-2)</f>
+      </c>
+      <c r="M33" s="5" t="str">
+        <f>INT(LEFT(L33,1))</f>
+      </c>
+      <c r="N33" s="5" t="str">
+        <f>RIGHT(L33,LEN(L33)-2)+0</f>
+      </c>
+      <c r="O33" s="5" t="str">
+        <f>K33*8*60+M33*60+N33</f>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="5" t="str">
+        <f>FLOOR(I29,1)&amp;"."&amp;(I29-FLOOR(I29,1))*8&amp;".0"</f>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K34" s="5" t="str">
+        <f>INT(LEFT(B35,1))</f>
+      </c>
+      <c r="L34" s="5" t="str">
+        <f>RIGHT(B35,LEN(B35)-2)</f>
+      </c>
+      <c r="M34" s="5" t="str">
+        <f>INT(LEFT(L34,1))</f>
+      </c>
+      <c r="N34" s="5" t="str">
+        <f>RIGHT(L34,LEN(L34)-2)+0</f>
+      </c>
+      <c r="O34" s="5" t="str">
+        <f>K34*8*60+M34*60+N34</f>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K35" s="5" t="str">
+        <f>INT(LEFT(B36,1))</f>
+      </c>
+      <c r="L35" s="5" t="str">
+        <f>RIGHT(B36,LEN(B36)-2)</f>
+      </c>
+      <c r="M35" s="5" t="str">
+        <f>INT(LEFT(L35,1))</f>
+      </c>
+      <c r="N35" s="5" t="str">
+        <f>RIGHT(L35,LEN(L35)-2)+0</f>
+      </c>
+      <c r="O35" s="5" t="str">
+        <f>K35*8*60+M35*60+N35</f>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K36" s="5" t="str">
+        <f>K31+IF(K32&gt;K34,K32-K34,0)+IF(K33&gt;K35,K33-K35,0)</f>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M36" s="5" t="str">
+        <f>M31+IF(M32&gt;M34,M32-M34,0)+IF(M33&gt;M35,M33-M35,0)</f>
+      </c>
+      <c r="N36" s="5" t="str">
+        <f>N31+IF(N32&gt;N34,N32-N34,0)+IF(N33&gt;N35,N33-N35,0)</f>
+      </c>
+      <c r="O36" s="5" t="str">
+        <f>O31+IF(O32&gt;O34,O32-O34,0)+IF(O33&gt;O35,O33-O35,0)</f>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <f>FLOOR(K37/8,1)&amp;"."&amp;FLOOR(MOD(K37,8),1)&amp;"."&amp;(MOD(K37,8)-FLOOR(MOD(K37,8),1))*60</f>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K37" s="5" t="str">
+        <f>O36/60</f>
       </c>
     </row>
   </sheetData>
@@ -1127,13 +1477,13 @@
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>